<commit_message>
Todo arreglado, falta lo de franco. Creo
</commit_message>
<xml_diff>
--- a/Sprint 2/Reunión Retrospectiva 2.xlsx
+++ b/Sprint 2/Reunión Retrospectiva 2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Proyecto</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>CookBook</t>
+  </si>
+  <si>
+    <t>Github anduvo bien toda la semana hasta el ultimo momento</t>
+  </si>
+  <si>
+    <t>primero hacer commit y dspues sincronizar</t>
+  </si>
+  <si>
+    <t>la idea es no tocar lo mismo</t>
+  </si>
+  <si>
+    <t>mejorar github</t>
   </si>
 </sst>
 </file>
@@ -539,7 +551,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -561,21 +573,29 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
clone y hago commit
</commit_message>
<xml_diff>
--- a/Sprint 2/Reunión Retrospectiva 2.xlsx
+++ b/Sprint 2/Reunión Retrospectiva 2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Proyecto</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>CookBook</t>
+  </si>
+  <si>
+    <t>Github anduvo bien toda la semana hasta el ultimo momento</t>
+  </si>
+  <si>
+    <t>primero hacer commit y dspues sincronizar</t>
+  </si>
+  <si>
+    <t>la idea es no tocar lo mismo</t>
+  </si>
+  <si>
+    <t>mejorar github</t>
   </si>
 </sst>
 </file>
@@ -539,7 +551,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -561,21 +573,29 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1">

</xml_diff>